<commit_message>
add SVC and DBN test
</commit_message>
<xml_diff>
--- a/raw_data/all.xlsx
+++ b/raw_data/all.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="155">
   <si>
     <t>id</t>
   </si>
@@ -450,28 +450,6 @@
     <t>18D</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3..7</t>
-    </r>
-  </si>
-  <si>
     <t>2D</t>
   </si>
   <si>
@@ -833,9 +811,6 @@
     </r>
   </si>
   <si>
-    <t>混合性</t>
-  </si>
-  <si>
     <t>13D+</t>
   </si>
   <si>
@@ -871,28 +846,6 @@
   </si>
   <si>
     <t>62D</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>..11</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1049,11 +1002,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1120,6 +1073,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1135,14 +1095,99 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1157,37 +1202,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -1195,69 +1209,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1296,7 +1249,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1308,13 +1327,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1326,61 +1393,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1392,91 +1423,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1626,8 +1579,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1647,15 +1600,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1671,12 +1615,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1699,24 +1665,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1724,148 +1677,148 @@
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2346,8 +2299,8 @@
   <sheetPr/>
   <dimension ref="A1:AM614"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AG13" sqref="AG13"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="P286" workbookViewId="0">
+      <selection activeCell="AD332" sqref="AD332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -21126,7 +21079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" ht="17" spans="1:38">
+    <row r="171" spans="1:38">
       <c r="A171" s="5">
         <v>166</v>
       </c>
@@ -21186,8 +21139,8 @@
       <c r="U171" s="5">
         <v>67.4</v>
       </c>
-      <c r="V171" s="5" t="s">
-        <v>93</v>
+      <c r="V171" s="5">
+        <v>23.7</v>
       </c>
       <c r="W171" s="5">
         <v>1</v>
@@ -21757,7 +21710,7 @@
         <v>1</v>
       </c>
       <c r="AB176" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AC176" s="20">
         <v>22</v>
@@ -21871,7 +21824,7 @@
         <v>1</v>
       </c>
       <c r="AB177" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AC177" s="20">
         <v>14</v>
@@ -22099,7 +22052,7 @@
         <v>1</v>
       </c>
       <c r="AB179" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AC179" s="20">
         <v>8</v>
@@ -22213,7 +22166,7 @@
         <v>1</v>
       </c>
       <c r="AB180" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC180" s="20">
         <v>30</v>
@@ -22435,7 +22388,7 @@
         <v>1</v>
       </c>
       <c r="AB182" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC182" s="20">
         <v>18</v>
@@ -22547,7 +22500,7 @@
         <v>1</v>
       </c>
       <c r="AB183" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC183" s="20">
         <v>4</v>
@@ -22663,7 +22616,7 @@
         <v>1</v>
       </c>
       <c r="AB184" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AC184" s="20">
         <v>25</v>
@@ -22891,7 +22844,7 @@
         <v>1</v>
       </c>
       <c r="AB186" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC186" s="20"/>
       <c r="AD186" s="20">
@@ -23003,7 +22956,7 @@
         <v>1</v>
       </c>
       <c r="AB187" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC187" s="20">
         <v>15</v>
@@ -23227,7 +23180,7 @@
         <v>1</v>
       </c>
       <c r="AB189" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AC189" s="20">
         <v>19</v>
@@ -24117,7 +24070,7 @@
         <v>1</v>
       </c>
       <c r="AB197" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AC197" s="20">
         <v>18</v>
@@ -24229,7 +24182,7 @@
         <v>1</v>
       </c>
       <c r="AB198" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC198" s="20">
         <v>25</v>
@@ -24799,7 +24752,7 @@
         <v>1</v>
       </c>
       <c r="AB203" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC203" s="20">
         <v>5</v>
@@ -24911,7 +24864,7 @@
         <v>1</v>
       </c>
       <c r="AB204" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC204" s="20">
         <v>24</v>
@@ -25359,7 +25312,7 @@
         <v>1</v>
       </c>
       <c r="AB208" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC208" s="20">
         <v>10</v>
@@ -25473,7 +25426,7 @@
         <v>1</v>
       </c>
       <c r="AB209" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC209" s="20">
         <v>9</v>
@@ -26263,7 +26216,7 @@
         <v>1</v>
       </c>
       <c r="AB216" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC216" s="20">
         <v>8</v>
@@ -26935,7 +26888,7 @@
         <v>1</v>
       </c>
       <c r="AB222" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC222" s="20">
         <v>20</v>
@@ -27039,7 +26992,7 @@
         <v>1</v>
       </c>
       <c r="AB223" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC223" s="20">
         <v>6</v>
@@ -29823,7 +29776,7 @@
         <v>1</v>
       </c>
       <c r="AB248" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AC248" s="20">
         <v>50</v>
@@ -29939,7 +29892,7 @@
         <v>1</v>
       </c>
       <c r="AB249" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC249" s="20">
         <v>22</v>
@@ -30055,7 +30008,7 @@
         <v>1</v>
       </c>
       <c r="AB250" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC250" s="20">
         <v>50</v>
@@ -30171,7 +30124,7 @@
         <v>1</v>
       </c>
       <c r="AB251" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC251" s="20">
         <v>20</v>
@@ -30287,7 +30240,7 @@
         <v>1</v>
       </c>
       <c r="AB252" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AC252" s="20">
         <v>70</v>
@@ -30403,7 +30356,7 @@
         <v>1</v>
       </c>
       <c r="AB253" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC253" s="20">
         <v>8</v>
@@ -30664,7 +30617,7 @@
         <v>0</v>
       </c>
       <c r="AM255" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="256" spans="1:38">
@@ -30746,7 +30699,7 @@
         <v>1</v>
       </c>
       <c r="AB256" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC256" s="20">
         <v>6</v>
@@ -30972,7 +30925,7 @@
         <v>1</v>
       </c>
       <c r="AB258" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC258" s="20">
         <v>14</v>
@@ -31084,7 +31037,7 @@
         <v>1</v>
       </c>
       <c r="AB259" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC259" s="20">
         <v>80</v>
@@ -31198,7 +31151,7 @@
         <v>1</v>
       </c>
       <c r="AB260" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AC260" s="20">
         <v>18</v>
@@ -31310,7 +31263,7 @@
         <v>1</v>
       </c>
       <c r="AB261" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC261" s="20">
         <v>81</v>
@@ -31414,7 +31367,7 @@
         <v>1</v>
       </c>
       <c r="AB262" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC262" s="20">
         <v>71</v>
@@ -31752,7 +31705,7 @@
         <v>1</v>
       </c>
       <c r="AB265" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AC265" s="20">
         <v>55</v>
@@ -31864,7 +31817,7 @@
         <v>1</v>
       </c>
       <c r="AB266" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC266" s="20">
         <v>4</v>
@@ -31980,7 +31933,7 @@
         <v>1</v>
       </c>
       <c r="AB267" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC267" s="20">
         <v>46</v>
@@ -32316,7 +32269,7 @@
         <v>1</v>
       </c>
       <c r="AB270" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC270" s="20">
         <v>24</v>
@@ -32546,7 +32499,7 @@
         <v>1</v>
       </c>
       <c r="AB272" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC272" s="20">
         <v>20</v>
@@ -32579,7 +32532,7 @@
         <v>0</v>
       </c>
       <c r="AM272" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="273" spans="1:38">
@@ -32637,7 +32590,7 @@
         <v>1</v>
       </c>
       <c r="AB273" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC273" s="20">
         <v>4</v>
@@ -33411,7 +33364,7 @@
         <v>1</v>
       </c>
       <c r="AB280" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC280" s="20">
         <v>9</v>
@@ -33523,7 +33476,7 @@
         <v>1</v>
       </c>
       <c r="AB281" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC281" s="20">
         <v>15</v>
@@ -33855,7 +33808,7 @@
         <v>1</v>
       </c>
       <c r="AB284" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC284" s="20">
         <v>14</v>
@@ -33965,7 +33918,7 @@
         <v>1</v>
       </c>
       <c r="AB285" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC285" s="20">
         <v>18</v>
@@ -34077,7 +34030,7 @@
         <v>1</v>
       </c>
       <c r="AB286" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC286" s="20">
         <v>19</v>
@@ -34189,7 +34142,7 @@
         <v>1</v>
       </c>
       <c r="AB287" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC287" s="20">
         <v>6</v>
@@ -34411,7 +34364,7 @@
         <v>1</v>
       </c>
       <c r="AB289" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC289" s="20">
         <v>5</v>
@@ -34865,7 +34818,7 @@
         <v>1</v>
       </c>
       <c r="AB293" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC293" s="20">
         <v>88</v>
@@ -35427,7 +35380,7 @@
         <v>1</v>
       </c>
       <c r="AB298" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC298" s="20">
         <v>19</v>
@@ -35539,7 +35492,7 @@
         <v>1</v>
       </c>
       <c r="AB299" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC299" s="20">
         <v>13</v>
@@ -35627,7 +35580,7 @@
         <v>1</v>
       </c>
       <c r="AB300" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AC300" s="20">
         <v>24</v>
@@ -35739,7 +35692,7 @@
         <v>1</v>
       </c>
       <c r="AB301" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AC301" s="20">
         <v>8</v>
@@ -36401,7 +36354,7 @@
         <v>1</v>
       </c>
       <c r="AB307" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC307" s="20">
         <v>16</v>
@@ -36957,7 +36910,7 @@
         <v>1</v>
       </c>
       <c r="AB312" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC312" s="20">
         <v>50</v>
@@ -37177,7 +37130,7 @@
         <v>1</v>
       </c>
       <c r="AB314" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC314" s="20">
         <v>23</v>
@@ -37291,7 +37244,7 @@
         <v>1</v>
       </c>
       <c r="AB315" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC315" s="20">
         <v>21</v>
@@ -37743,7 +37696,7 @@
         <v>1</v>
       </c>
       <c r="AB319" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC319" s="20">
         <v>18</v>
@@ -37969,7 +37922,7 @@
         <v>1</v>
       </c>
       <c r="AB321" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AC321" s="20">
         <v>28</v>
@@ -38191,7 +38144,7 @@
         <v>1</v>
       </c>
       <c r="AB323" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC323" s="20">
         <v>26</v>
@@ -38305,7 +38258,7 @@
         <v>1</v>
       </c>
       <c r="AB324" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC324" s="20">
         <v>14</v>
@@ -38863,7 +38816,7 @@
         <v>1</v>
       </c>
       <c r="AB329" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC329" s="20">
         <v>13</v>
@@ -39193,7 +39146,7 @@
         <v>1</v>
       </c>
       <c r="AB332" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC332" s="20">
         <v>30</v>
@@ -39650,9 +39603,7 @@
       <c r="AC336" s="20">
         <v>48</v>
       </c>
-      <c r="AD336" s="20" t="s">
-        <v>132</v>
-      </c>
+      <c r="AD336" s="20"/>
       <c r="AE336" s="20">
         <v>2</v>
       </c>
@@ -39875,7 +39826,7 @@
         <v>1</v>
       </c>
       <c r="AB338" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC338" s="20">
         <v>9</v>
@@ -40215,7 +40166,7 @@
         <v>1</v>
       </c>
       <c r="AB341" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC341" s="20">
         <v>4</v>
@@ -40327,7 +40278,7 @@
         <v>1</v>
       </c>
       <c r="AB342" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AC342" s="20">
         <v>11</v>
@@ -41449,7 +41400,7 @@
         <v>1</v>
       </c>
       <c r="AB352" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC352" s="20">
         <v>19</v>
@@ -41895,7 +41846,7 @@
         <v>1</v>
       </c>
       <c r="AB356" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC356" s="20">
         <v>5</v>
@@ -42345,7 +42296,7 @@
         <v>1</v>
       </c>
       <c r="AB360" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC360" s="20">
         <v>36</v>
@@ -42569,7 +42520,7 @@
         <v>1</v>
       </c>
       <c r="AB362" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC362" s="20">
         <v>10</v>
@@ -42681,7 +42632,7 @@
         <v>1</v>
       </c>
       <c r="AB363" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AC363" s="20">
         <v>9</v>
@@ -43125,7 +43076,7 @@
         <v>1</v>
       </c>
       <c r="AB367" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AC367" s="20">
         <v>14</v>
@@ -43241,7 +43192,7 @@
         <v>1</v>
       </c>
       <c r="AB368" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AC368" s="20">
         <v>21</v>
@@ -43989,7 +43940,7 @@
         <v>1</v>
       </c>
       <c r="AB375" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC375" s="20">
         <v>34</v>
@@ -44101,7 +44052,7 @@
         <v>1</v>
       </c>
       <c r="AB376" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AC376" s="20">
         <v>95</v>
@@ -44213,7 +44164,7 @@
         <v>1</v>
       </c>
       <c r="AB377" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AC377" s="20">
         <v>74</v>
@@ -44435,7 +44386,7 @@
         <v>1</v>
       </c>
       <c r="AB379" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC379" s="20"/>
       <c r="AD379" s="20">
@@ -44657,7 +44608,7 @@
         <v>1</v>
       </c>
       <c r="AB381" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC381" s="20">
         <v>73</v>
@@ -44773,7 +44724,7 @@
         <v>1</v>
       </c>
       <c r="AB382" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC382" s="20">
         <v>83</v>
@@ -45329,7 +45280,7 @@
         <v>1</v>
       </c>
       <c r="AB387" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AC387" s="20">
         <v>55</v>
@@ -45443,7 +45394,7 @@
         <v>1</v>
       </c>
       <c r="AB388" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC388" s="20">
         <v>39</v>
@@ -45559,7 +45510,7 @@
         <v>1</v>
       </c>
       <c r="AB389" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC389" s="20">
         <v>68</v>
@@ -45750,8 +45701,8 @@
       <c r="O391" s="5">
         <v>181</v>
       </c>
-      <c r="P391" s="5" t="s">
-        <v>139</v>
+      <c r="P391" s="5">
+        <v>3.11</v>
       </c>
       <c r="Q391" s="16"/>
       <c r="R391" s="16"/>
@@ -45783,7 +45734,7 @@
         <v>1</v>
       </c>
       <c r="AB391" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AC391" s="20">
         <v>53</v>
@@ -45899,7 +45850,7 @@
         <v>1</v>
       </c>
       <c r="AB392" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC392" s="20">
         <v>26</v>
@@ -48545,7 +48496,7 @@
         <v>1</v>
       </c>
       <c r="AB416" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AC416" s="20">
         <v>24</v>
@@ -48657,7 +48608,7 @@
         <v>1</v>
       </c>
       <c r="AB417" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC417" s="20">
         <v>48</v>
@@ -49109,7 +49060,7 @@
         <v>1</v>
       </c>
       <c r="AB421" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AC421" s="20">
         <v>18</v>
@@ -49339,7 +49290,7 @@
         <v>1</v>
       </c>
       <c r="AB423" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC423" s="20">
         <v>80</v>
@@ -49675,7 +49626,7 @@
         <v>1</v>
       </c>
       <c r="AB426" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC426" s="20"/>
       <c r="AD426" s="20">
@@ -49789,7 +49740,7 @@
         <v>1</v>
       </c>
       <c r="AB427" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC427" s="20"/>
       <c r="AD427" s="20">
@@ -49899,7 +49850,7 @@
         <v>1</v>
       </c>
       <c r="AB428" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC428" s="20">
         <v>105</v>
@@ -50015,7 +49966,7 @@
         <v>1</v>
       </c>
       <c r="AB429" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AC429" s="20">
         <v>116</v>
@@ -50581,7 +50532,7 @@
         <v>1</v>
       </c>
       <c r="AB434" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC434" s="20"/>
       <c r="AD434" s="20">
@@ -50805,7 +50756,7 @@
         <v>1</v>
       </c>
       <c r="AB436" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AC436" s="20">
         <v>61</v>
@@ -50915,7 +50866,7 @@
         <v>1</v>
       </c>
       <c r="AB437" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AC437" s="20">
         <v>56</v>
@@ -51661,7 +51612,7 @@
         <v>1</v>
       </c>
       <c r="AB444" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AC444" s="20">
         <v>60</v>
@@ -52117,7 +52068,7 @@
         <v>1</v>
       </c>
       <c r="AB448" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC448" s="20">
         <v>83</v>
@@ -53565,7 +53516,7 @@
         <v>1</v>
       </c>
       <c r="AB461" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AC461" s="20">
         <v>53</v>
@@ -53681,7 +53632,7 @@
         <v>1</v>
       </c>
       <c r="AB462" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AC462" s="20">
         <v>43</v>
@@ -53793,7 +53744,7 @@
         <v>1</v>
       </c>
       <c r="AB463" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC463" s="20">
         <v>78</v>
@@ -54365,7 +54316,7 @@
         <v>1</v>
       </c>
       <c r="AB468" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC468" s="20">
         <v>66</v>
@@ -54477,7 +54428,7 @@
         <v>1</v>
       </c>
       <c r="AB469" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AC469" s="20">
         <v>90</v>
@@ -54589,7 +54540,7 @@
         <v>1</v>
       </c>
       <c r="AB470" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AC470" s="20">
         <v>60</v>
@@ -54703,7 +54654,7 @@
         <v>1</v>
       </c>
       <c r="AB471" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC471" s="20">
         <v>26</v>
@@ -54817,7 +54768,7 @@
         <v>1</v>
       </c>
       <c r="AB472" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AC472" s="20">
         <v>65</v>
@@ -55153,7 +55104,7 @@
         <v>1</v>
       </c>
       <c r="AB475" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC475" s="20">
         <v>65</v>
@@ -55493,7 +55444,7 @@
         <v>1</v>
       </c>
       <c r="AB478" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AC478" s="20">
         <v>45</v>
@@ -55605,7 +55556,7 @@
         <v>1</v>
       </c>
       <c r="AB479" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AC479" s="20">
         <v>43</v>
@@ -56169,7 +56120,7 @@
         <v>1</v>
       </c>
       <c r="AB484" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC484" s="20">
         <v>81</v>
@@ -56609,7 +56560,7 @@
         <v>1</v>
       </c>
       <c r="AB488" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AC488" s="20">
         <v>60</v>
@@ -56833,7 +56784,7 @@
         <v>1</v>
       </c>
       <c r="AB490" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC490" s="20">
         <v>80</v>
@@ -57689,7 +57640,7 @@
         <v>1</v>
       </c>
       <c r="AB498" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC498" s="20">
         <v>91</v>
@@ -57917,7 +57868,7 @@
         <v>1</v>
       </c>
       <c r="AB500" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC500" s="20">
         <v>69</v>
@@ -58031,7 +57982,7 @@
         <v>1</v>
       </c>
       <c r="AB501" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC501" s="20">
         <v>71</v>
@@ -58145,7 +58096,7 @@
         <v>1</v>
       </c>
       <c r="AB502" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC502" s="20">
         <v>99</v>
@@ -58711,7 +58662,7 @@
         <v>1</v>
       </c>
       <c r="AB507" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC507" s="20">
         <v>51</v>
@@ -58913,7 +58864,7 @@
         <v>1</v>
       </c>
       <c r="AB509" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC509" s="20">
         <v>64</v>
@@ -59141,7 +59092,7 @@
         <v>1</v>
       </c>
       <c r="AB511" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AC511" s="20">
         <v>85</v>
@@ -59229,7 +59180,7 @@
         <v>1</v>
       </c>
       <c r="AB512" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC512" s="20"/>
       <c r="AD512" s="20">
@@ -59339,7 +59290,7 @@
         <v>1</v>
       </c>
       <c r="AB513" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AC513" s="20">
         <v>66</v>
@@ -59453,7 +59404,7 @@
         <v>1</v>
       </c>
       <c r="AB514" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AC514" s="20">
         <v>79</v>
@@ -59681,7 +59632,7 @@
         <v>1</v>
       </c>
       <c r="AB516" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AC516" s="20">
         <v>88</v>
@@ -60127,7 +60078,7 @@
         <v>1</v>
       </c>
       <c r="AB520" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC520" s="20">
         <v>96</v>
@@ -60239,7 +60190,7 @@
         <v>1</v>
       </c>
       <c r="AB521" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC521" s="20"/>
       <c r="AD521" s="20">
@@ -60351,7 +60302,7 @@
         <v>1</v>
       </c>
       <c r="AB522" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AC522" s="20"/>
       <c r="AD522" s="20">
@@ -60565,7 +60516,7 @@
         <v>1</v>
       </c>
       <c r="AB524" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AC524" s="20">
         <v>75</v>
@@ -60679,7 +60630,7 @@
         <v>1</v>
       </c>
       <c r="AB525" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AC525" s="20">
         <v>99</v>
@@ -60791,7 +60742,7 @@
         <v>1</v>
       </c>
       <c r="AB526" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AC526" s="20">
         <v>108</v>
@@ -61037,7 +60988,7 @@
         <v>67</v>
       </c>
       <c r="D529" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E529" s="5">
         <v>2</v>
@@ -61147,7 +61098,7 @@
         <v>19</v>
       </c>
       <c r="D530" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E530" s="5">
         <v>2</v>
@@ -61215,7 +61166,7 @@
         <v>1</v>
       </c>
       <c r="AB530" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AC530" s="20">
         <v>78</v>
@@ -61259,7 +61210,7 @@
         <v>45</v>
       </c>
       <c r="D531" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E531" s="5">
         <v>1</v>
@@ -61369,7 +61320,7 @@
         <v>64</v>
       </c>
       <c r="D532" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E532" s="5">
         <v>2</v>
@@ -61485,7 +61436,7 @@
         <v>56</v>
       </c>
       <c r="D533" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E533" s="5">
         <v>0</v>
@@ -61779,7 +61730,7 @@
         <v>1</v>
       </c>
       <c r="AB535" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AC535" s="20"/>
       <c r="AD535" s="20">
@@ -63437,7 +63388,7 @@
         <v>1</v>
       </c>
       <c r="AB550" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC550" s="20"/>
       <c r="AD550" s="20">
@@ -64331,7 +64282,7 @@
         <v>1</v>
       </c>
       <c r="AB558" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC558" s="20">
         <v>80</v>
@@ -64887,7 +64838,7 @@
         <v>1</v>
       </c>
       <c r="AB563" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC563" s="20">
         <v>110</v>
@@ -65001,7 +64952,7 @@
         <v>1</v>
       </c>
       <c r="AB564" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC564" s="20">
         <v>88</v>
@@ -65219,7 +65170,7 @@
         <v>1</v>
       </c>
       <c r="AB566" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC566" s="20"/>
       <c r="AD566" s="20">
@@ -65663,7 +65614,7 @@
         <v>1</v>
       </c>
       <c r="AB570" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AC570" s="20">
         <v>63</v>
@@ -65889,7 +65840,7 @@
         <v>1</v>
       </c>
       <c r="AB572" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC572" s="20"/>
       <c r="AD572" s="20">
@@ -66227,7 +66178,7 @@
         <v>1</v>
       </c>
       <c r="AB575" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AC575" s="20"/>
       <c r="AD575" s="20">
@@ -66337,7 +66288,7 @@
         <v>1</v>
       </c>
       <c r="AB576" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC576" s="20"/>
       <c r="AD576" s="20">
@@ -66715,7 +66666,7 @@
         <v>81</v>
       </c>
       <c r="D580" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E580" s="5">
         <v>2</v>
@@ -67003,7 +66954,7 @@
         <v>1</v>
       </c>
       <c r="AB582" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC582" s="20">
         <v>74</v>
@@ -67117,7 +67068,7 @@
         <v>1</v>
       </c>
       <c r="AB583" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC583" s="20">
         <v>70</v>
@@ -67679,7 +67630,7 @@
         <v>1</v>
       </c>
       <c r="AB588" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC588" s="20">
         <v>41</v>
@@ -68349,7 +68300,7 @@
         <v>1</v>
       </c>
       <c r="AB594" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC594" s="20">
         <v>85</v>
@@ -68907,7 +68858,7 @@
         <v>1</v>
       </c>
       <c r="AB599" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC599" s="20">
         <v>90</v>
@@ -69245,7 +69196,7 @@
         <v>1</v>
       </c>
       <c r="AB602" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC602" s="20">
         <v>70</v>
@@ -70021,7 +69972,7 @@
         <v>1</v>
       </c>
       <c r="AB609" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AC609" s="20">
         <v>110</v>
@@ -70357,7 +70308,7 @@
         <v>1</v>
       </c>
       <c r="AB612" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC612" s="20">
         <v>108</v>
@@ -70401,7 +70352,7 @@
         <v>84</v>
       </c>
       <c r="D613" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E613" s="5">
         <v>2</v>
@@ -70583,7 +70534,7 @@
         <v>1</v>
       </c>
       <c r="AB614" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC614" s="20"/>
       <c r="AD614" s="20"/>

</xml_diff>

<commit_message>
Fix errors in source data
</commit_message>
<xml_diff>
--- a/raw_data/all.xlsx
+++ b/raw_data/all.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="19240"/>
+    <workbookView windowHeight="18200"/>
   </bookViews>
   <sheets>
     <sheet name="原始数据" sheetId="1" r:id="rId1"/>
@@ -1000,12 +1000,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="28">
@@ -1072,30 +1072,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1103,7 +1082,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1117,26 +1096,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1157,6 +1120,45 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
@@ -1165,7 +1167,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1180,6 +1182,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1187,30 +1203,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1249,25 +1249,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1279,79 +1267,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1369,7 +1297,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1381,55 +1387,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1576,15 +1576,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1600,17 +1591,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1630,20 +1624,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1665,6 +1656,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1676,151 +1676,151 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1828,74 +1828,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="49" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="49" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="49" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="49" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="49" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="49" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1916,85 +1916,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="2" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="3" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="4" builtinId="41"/>
-    <cellStyle name="输入" xfId="5" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="7" builtinId="38"/>
-    <cellStyle name="货币" xfId="8" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="9" builtinId="37"/>
-    <cellStyle name="百分比" xfId="10" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="11" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="12" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="13" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="14" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="15" builtinId="44"/>
-    <cellStyle name="计算" xfId="16" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="17" builtinId="29"/>
-    <cellStyle name="适中" xfId="18" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="19" builtinId="46"/>
-    <cellStyle name="好" xfId="20" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="21" builtinId="30"/>
-    <cellStyle name="汇总" xfId="22" builtinId="25"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
     <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="24" builtinId="23"/>
-    <cellStyle name="输出" xfId="25" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="26" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="27" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="28" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="29" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="30" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="31" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="32" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="33" builtinId="9"/>
-    <cellStyle name="标题" xfId="34" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="35" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="36" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="37" builtinId="40"/>
-    <cellStyle name="注释" xfId="38" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="40" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="41" builtinId="51"/>
-    <cellStyle name="超链接" xfId="42" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="43" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="44" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="45" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="46" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="48" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="49" builtinId="24"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规 2" xfId="49"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
@@ -2299,8 +2299,8 @@
   <sheetPr/>
   <dimension ref="A1:AM614"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="P286" workbookViewId="0">
-      <selection activeCell="AD332" sqref="AD332"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A351" workbookViewId="0">
+      <selection activeCell="R400" sqref="R400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -46592,17 +46592,16 @@
       <c r="L399" s="5">
         <v>1</v>
       </c>
-      <c r="M399" s="5"/>
+      <c r="M399" s="5">
+        <v>9.46</v>
+      </c>
       <c r="N399" s="5">
-        <v>9.46</v>
-      </c>
-      <c r="O399" s="5">
         <v>131</v>
       </c>
-      <c r="P399" s="14">
+      <c r="O399" s="14">
         <v>358</v>
       </c>
-      <c r="Q399" s="5">
+      <c r="P399" s="5">
         <v>2.47</v>
       </c>
       <c r="R399" s="5"/>

</xml_diff>